<commit_message>
working for multiple "display" sheets
</commit_message>
<xml_diff>
--- a/excel_template_shiny.xlsx
+++ b/excel_template_shiny.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lclem\OneDrive\Documents\GitHub\plhR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F097614E-BE39-4D8C-8798-03F303ADE8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D1BF24-1BD3-4D1E-AC0B-AD01D638DAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="2" r:id="rId1"/>
     <sheet name="main_page" sheetId="3" r:id="rId2"/>
     <sheet name="demographics" sheetId="1" r:id="rId3"/>
+    <sheet name="demo2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="33">
   <si>
     <t>type</t>
   </si>
@@ -115,6 +116,12 @@
   </si>
   <si>
     <t>users</t>
+  </si>
+  <si>
+    <t>TestTab</t>
+  </si>
+  <si>
+    <t>demo2</t>
   </si>
 </sst>
 </file>
@@ -501,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870FAA04-D1DA-469D-A43D-8817AEA92C36}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -538,6 +545,20 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -562,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,6 +593,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -671,6 +695,194 @@
       </c>
       <c r="E6" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6B29A1-47D6-45AF-A780-81A3867471CA}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
icon amendments in template
</commit_message>
<xml_diff>
--- a/excel_template_shiny.xlsx
+++ b/excel_template_shiny.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lclem\OneDrive\Documents\GitHub\plhR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC961E19-46DC-40BB-9331-5838A5B863E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07234321-A933-48C3-9D29-0E3671BA0BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,21 +121,9 @@
     <t>value_box</t>
   </si>
   <si>
-    <t>text = "Consented", colour = "aqua", icon = "user"</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>text = "Active users", colour = "purple", icon = "user"</t>
-  </si>
-  <si>
-    <t>text = "In program", colour = "green", icon = "clock"</t>
-  </si>
-  <si>
-    <t>text = "Total", colour = "yellow", icon = "calendar"</t>
-  </si>
-  <si>
     <t>active_users_24_hrs</t>
   </si>
   <si>
@@ -155,6 +143,18 @@
   </si>
   <si>
     <t>myvaluebox4</t>
+  </si>
+  <si>
+    <t>text = "Active in last 24 hours", colour = "purple", icon = "clock"</t>
+  </si>
+  <si>
+    <t>text = "Active in last 7 days", colour = "green", icon = "calendar"</t>
+  </si>
+  <si>
+    <t>text = "Total", colour = "yellow", icon = "user"</t>
+  </si>
+  <si>
+    <t>text = "Consented", colour = "aqua", icon = "clipboard"</t>
   </si>
 </sst>
 </file>
@@ -621,7 +621,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -658,13 +658,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -672,16 +672,16 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -689,16 +689,16 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -706,16 +706,16 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding new functions for tabbed_display
</commit_message>
<xml_diff>
--- a/excel_template_shiny.xlsx
+++ b/excel_template_shiny.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lclem\OneDrive\Documents\GitHub\plhR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01E631C-F9A9-409C-9062-7ED3AD8E1E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC271AE-E3AE-4509-B147-239B1E9A5A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="731" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="2" r:id="rId1"/>
@@ -18,14 +18,16 @@
     <sheet name="demographics" sheetId="1" r:id="rId3"/>
     <sheet name="demo2" sheetId="4" r:id="rId4"/>
     <sheet name="download" sheetId="5" r:id="rId5"/>
-    <sheet name="tabbed_display_ajdkds" sheetId="6" r:id="rId6"/>
+    <sheet name="td_engagement" sheetId="6" r:id="rId6"/>
+    <sheet name="td_eng_overview" sheetId="7" r:id="rId7"/>
+    <sheet name="td_eng_insights" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="61">
   <si>
     <t>type</t>
   </si>
@@ -162,18 +164,6 @@
     <t>download</t>
   </si>
   <si>
-    <t>main_tab</t>
-  </si>
-  <si>
-    <t>tab_page</t>
-  </si>
-  <si>
-    <t>One</t>
-  </si>
-  <si>
-    <t>Two</t>
-  </si>
-  <si>
     <t>Data label</t>
   </si>
   <si>
@@ -199,6 +189,27 @@
   </si>
   <si>
     <t>Demo2</t>
+  </si>
+  <si>
+    <t>Engagement</t>
+  </si>
+  <si>
+    <t>lightbulb</t>
+  </si>
+  <si>
+    <t>td_engagement</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Additional Insights</t>
+  </si>
+  <si>
+    <t>td_eng_overview</t>
+  </si>
+  <si>
+    <t>td_eng_insights</t>
   </si>
 </sst>
 </file>
@@ -593,13 +604,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870FAA04-D1DA-469D-A43D-8817AEA92C36}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -660,8 +673,17 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
       <c r="B5" t="s">
         <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -781,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -894,7 +916,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G4" sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1026,15 +1048,15 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -1042,32 +1064,32 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1077,15 +1099,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0ED4D7-E189-430E-8A87-00F28BD4FBE8}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1100,24 +1124,221 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD3C195-BC6A-425E-8EEC-3F078ED6F497}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63356379-451F-4BA1-BFC6-602CACF0A5E7}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>